<commit_message>
Asteroid fields work now.
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Priority</t>
   </si>
@@ -123,14 +123,28 @@
   </si>
   <si>
     <t>Soft boundary</t>
+  </si>
+  <si>
+    <t>Bullets</t>
+  </si>
+  <si>
+    <t>Blast particles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -179,9 +193,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:I261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f>E7*F7</f>
+        <f t="shared" ref="G7:G22" si="0">E7*F7</f>
         <v>1</v>
       </c>
       <c r="H7" s="1"/>
@@ -543,18 +558,18 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f>E8*F8</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8">
-        <f t="shared" ref="I8:I22" si="0">E8*H8</f>
+        <f t="shared" ref="I8:I22" si="1">E8*H8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" ref="A9:A72" si="1">A8-1</f>
+        <f t="shared" ref="A9:A72" si="2">A8-1</f>
         <v>253</v>
       </c>
       <c r="C9">
@@ -564,25 +579,25 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E22" si="2">E8*2</f>
+        <f t="shared" ref="E9:E22" si="3">E8*2</f>
         <v>4</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9">
-        <f>E9*F9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>252</v>
       </c>
       <c r="C10">
@@ -592,27 +607,27 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10">
-        <f>E10*F10</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="C11">
@@ -622,25 +637,25 @@
         <v>6</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11">
-        <f>E11*F11</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="C12">
@@ -650,25 +665,25 @@
         <v>9</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12">
-        <f>E12*F12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>249</v>
       </c>
       <c r="C13">
@@ -678,25 +693,25 @@
         <v>10</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
       <c r="G13">
-        <f>E13*F13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248</v>
       </c>
       <c r="C14">
@@ -706,25 +721,25 @@
         <v>5</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14">
-        <f>E14*F14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>247</v>
       </c>
       <c r="C15">
@@ -734,25 +749,25 @@
         <v>7</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
       </c>
       <c r="G15">
-        <f>E15*F15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>246</v>
       </c>
       <c r="C16">
@@ -762,25 +777,25 @@
         <v>8</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>512</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
       <c r="G16">
-        <f>E16*F16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>245</v>
       </c>
       <c r="C17">
@@ -790,25 +805,25 @@
         <v>21</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1024</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17">
-        <f>E17*F17</f>
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244</v>
       </c>
       <c r="C18">
@@ -818,25 +833,25 @@
         <v>16</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2048</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
       </c>
       <c r="G18">
-        <f>E18*F18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>243</v>
       </c>
       <c r="C19">
@@ -846,25 +861,25 @@
         <v>22</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4096</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
       </c>
       <c r="G19">
-        <f>E19*F19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>242</v>
       </c>
       <c r="C20">
@@ -874,25 +889,25 @@
         <v>24</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8192</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="G20">
-        <f>E20*F20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>241</v>
       </c>
       <c r="C21">
@@ -902,50 +917,50 @@
         <v>25</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16384</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f>E21*F21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="C22">
         <v>16</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32768</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
       <c r="G22">
-        <f>E22*F22</f>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>239</v>
       </c>
       <c r="F23" s="1"/>
@@ -953,7 +968,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>238</v>
       </c>
       <c r="F24" s="1">
@@ -967,133 +982,133 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="B46" t="s">
@@ -1102,145 +1117,145 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>213</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="B70" t="s">
@@ -1249,151 +1264,151 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" ref="A73:A136" si="3">A72-1</f>
+        <f t="shared" ref="A73:A136" si="4">A72-1</f>
         <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>186</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>184</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>177</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>176</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>174</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>167</v>
       </c>
       <c r="B95" t="s">
@@ -1402,124 +1417,131 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>166</v>
       </c>
       <c r="B96" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>164</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>163</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>162</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>159</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>154</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>153</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>152</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>151</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>149</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>148</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>147</v>
       </c>
       <c r="B115" t="s">
@@ -1528,55 +1550,55 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>146</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>145</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>144</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>143</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>141</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>139</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>138</v>
       </c>
       <c r="B124" t="s">
@@ -1585,61 +1607,61 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>137</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>135</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>133</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>132</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="B134" t="s">
@@ -1648,49 +1670,49 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
-        <f t="shared" ref="A137:A200" si="4">A136-1</f>
+        <f t="shared" ref="A137:A200" si="5">A136-1</f>
         <v>125</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>124</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>123</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>122</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="B142" t="s">
@@ -1699,85 +1721,85 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>118</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>117</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>115</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>114</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>113</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>111</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>109</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>107</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>106</v>
       </c>
       <c r="B156" t="s">
@@ -1786,409 +1808,409 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>105</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>103</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>102</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>101</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>96</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>94</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>93</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>91</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>69</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201">
-        <f t="shared" ref="A201:A261" si="5">A200-1</f>
+        <f t="shared" ref="A201:A261" si="6">A200-1</f>
         <v>61</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>52</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>51</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="B224" t="s">
@@ -2197,25 +2219,25 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="B228" t="s">
@@ -2224,25 +2246,25 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="B232" t="s">
@@ -2251,25 +2273,25 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="B236" t="s">
@@ -2278,151 +2300,151 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B261" t="s">
@@ -2431,5 +2453,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>